<commit_message>
Auswertung angefangen und Tabellen to Latex code fertig
</commit_message>
<xml_diff>
--- a/v103/tables/runderstabeinseitig.xlsx
+++ b/v103/tables/runderstabeinseitig.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobyt\OneDrive\Desktop\Praktikumsberichte\grundpraktikum\v103\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{8A0A82D0-DA42-44A6-A027-29A30FE544C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBF97C3-1EC3-4855-9A3B-BE3281498FED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11680" yWindow="6920" windowWidth="21120" windowHeight="14120"/>
+    <workbookView xWindow="3420" yWindow="1880" windowWidth="21120" windowHeight="14120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,15 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
   <si>
-    <t xml:space="preserve"> $x / 10^{-3} \unit\meter$</t>
-  </si>
-  <si>
-    <t>$D_0 (x) / 10^{-3} \unit\meter$</t>
-  </si>
-  <si>
-    <t>$D_m (x)/ 10^{-3} \unit\meter$</t>
-  </si>
-  <si>
     <t>0.00</t>
   </si>
   <si>
@@ -229,12 +220,21 @@
   </si>
   <si>
     <t>6.69</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $x / 10^{3} \unit\meter$</t>
+  </si>
+  <si>
+    <t>$D_0 (x) / 10^{3} \unit\meter$</t>
+  </si>
+  <si>
+    <t>$D_m (x)/ 10^{3} \unit\meter$</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -580,11 +580,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -594,13 +594,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -608,10 +608,10 @@
         <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -619,10 +619,10 @@
         <v>50</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -630,10 +630,10 @@
         <v>70</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -641,10 +641,10 @@
         <v>90</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -652,10 +652,10 @@
         <v>110</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -663,10 +663,10 @@
         <v>130</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -674,10 +674,10 @@
         <v>150</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -685,10 +685,10 @@
         <v>170</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -696,175 +696,175 @@
         <v>190</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>